<commit_message>
ADDED: explore models for all shaperatings
</commit_message>
<xml_diff>
--- a/temporary_files/highu_apps.xlsx
+++ b/temporary_files/highu_apps.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgarduron/Documents/Working-Papers/AppStore-Research/AppStore_Analysis/AppStore/temporary_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F0EC06-6632-AB4D-AA4A-98CB846FDC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692CBC5F-A66E-1744-A5C4-194F297460D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="500" windowWidth="20740" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1680" yWindow="-25160" windowWidth="27620" windowHeight="20800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="148">
   <si>
     <t>term</t>
   </si>
@@ -89,19 +90,524 @@
   </si>
   <si>
     <t>regulatory_focusPrevention:highU_exploredTRUE</t>
+  </si>
+  <si>
+    <t>Table 1. Purchase Behavior</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Logit-1</t>
+  </si>
+  <si>
+    <t>Logit-2</t>
+  </si>
+  <si>
+    <t>-4.650***
+(0.000)</t>
+  </si>
+  <si>
+    <t>-4.556***
+(0.000)</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>0.016
+(0.279)</t>
+  </si>
+  <si>
+    <t>0.019
+(0.194)</t>
+  </si>
+  <si>
+    <t>Gender (Female)</t>
+  </si>
+  <si>
+    <t>0.733**
+(0.006)</t>
+  </si>
+  <si>
+    <t>0.730**
+(0.007)</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>-0.008
+(0.922)</t>
+  </si>
+  <si>
+    <t>0.001
+(0.989)</t>
+  </si>
+  <si>
+    <t>Visit Frequency</t>
+  </si>
+  <si>
+    <t>0.514*
+(0.024)</t>
+  </si>
+  <si>
+    <t>0.590*
+(0.012)</t>
+  </si>
+  <si>
+    <t>App Expense</t>
+  </si>
+  <si>
+    <t>0.151
+(0.200)</t>
+  </si>
+  <si>
+    <t>0.141
+(0.232)</t>
+  </si>
+  <si>
+    <t>Previous Experience</t>
+  </si>
+  <si>
+    <t>0.034
+(0.749)</t>
+  </si>
+  <si>
+    <t>0.035
+(0.743)</t>
+  </si>
+  <si>
+    <t>RF (Prevention)</t>
+  </si>
+  <si>
+    <t>0.027
+(0.919)</t>
+  </si>
+  <si>
+    <t>-1.232*
+(0.014)</t>
+  </si>
+  <si>
+    <t>Platf. Pref. (AppStore)</t>
+  </si>
+  <si>
+    <t>-0.185
+(0.499)</t>
+  </si>
+  <si>
+    <t>-0.181
+(0.516)</t>
+  </si>
+  <si>
+    <t>Involvement (1)</t>
+  </si>
+  <si>
+    <t>-0.319
+(0.288)</t>
+  </si>
+  <si>
+    <t>-0.290
+(0.342)</t>
+  </si>
+  <si>
+    <t>HighU Explored (TRUE)</t>
+  </si>
+  <si>
+    <t>0.731**
+(0.008)</t>
+  </si>
+  <si>
+    <t>-0.122
+(0.745)</t>
+  </si>
+  <si>
+    <t>RF*HighUExplored</t>
+  </si>
+  <si>
+    <t>1.934**
+(0.002)</t>
+  </si>
+  <si>
+    <t>Notes. p &lt; 0.10; *p &lt; 0.05; **p &lt; 0.01; ***p &lt; 0.001</t>
+  </si>
+  <si>
+    <t>App Name (JogStats)</t>
+  </si>
+  <si>
+    <t>App Name (Map My Walk)</t>
+  </si>
+  <si>
+    <t>App Name (Running Watch)</t>
+  </si>
+  <si>
+    <t>App Order (2)</t>
+  </si>
+  <si>
+    <t>App Order (3)</t>
+  </si>
+  <si>
+    <t>App Order (4)</t>
+  </si>
+  <si>
+    <t>Notes. p &lt; 0.10; *p &lt; 0.05; **p &lt; 0.01; ***p &lt; 0.001. Logit-1 refers to HighU and Logit-2 refers to HighJ.</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>-4.892***
+(0.000)</t>
+  </si>
+  <si>
+    <t>0.357
+(0.357)</t>
+  </si>
+  <si>
+    <t>-0.098
+(0.818)</t>
+  </si>
+  <si>
+    <t>0.13
+(0.747)</t>
+  </si>
+  <si>
+    <t>0.107
+(0.788)</t>
+  </si>
+  <si>
+    <t>0.299
+(0.456)</t>
+  </si>
+  <si>
+    <t>0.015
+(0.332)</t>
+  </si>
+  <si>
+    <t>0.735**
+(0.009)</t>
+  </si>
+  <si>
+    <t>0.016
+(0.856)</t>
+  </si>
+  <si>
+    <t>0.577*
+(0.016)</t>
+  </si>
+  <si>
+    <t>0.148
+(0.220)</t>
+  </si>
+  <si>
+    <t>0.049
+(0.653)</t>
+  </si>
+  <si>
+    <t>-0.206
+(0.468)</t>
+  </si>
+  <si>
+    <t>-0.309
+(0.318)</t>
+  </si>
+  <si>
+    <t>-1.371**
+(0.007)</t>
+  </si>
+  <si>
+    <t>0.828*
+(0.026)</t>
+  </si>
+  <si>
+    <t>0.731
+(0.559)</t>
+  </si>
+  <si>
+    <t>2.189***
+(0.001)</t>
+  </si>
+  <si>
+    <t>-0.006
+(0.656)</t>
+  </si>
+  <si>
+    <t>0.02
+(0.777)</t>
+  </si>
+  <si>
+    <t>-0.009
+(0.919)</t>
+  </si>
+  <si>
+    <t>0.268
+(0.253)</t>
+  </si>
+  <si>
+    <t>0.003
+(0.991)</t>
+  </si>
+  <si>
+    <t>0.121
+(0.732)</t>
+  </si>
+  <si>
+    <t>-0.157
+(0.641)</t>
+  </si>
+  <si>
+    <t>-0.052
+(0.876)</t>
+  </si>
+  <si>
+    <t>-0.47
+(0.159)</t>
+  </si>
+  <si>
+    <t>0.101
+(0.757)</t>
+  </si>
+  <si>
+    <t>Logit-3</t>
+  </si>
+  <si>
+    <t>Logit-4</t>
+  </si>
+  <si>
+    <t>-0.004
+(0.814)</t>
+  </si>
+  <si>
+    <t>-0.059
+(0.545)</t>
+  </si>
+  <si>
+    <t>0.131
+(0.611)</t>
+  </si>
+  <si>
+    <t>0.160
+(0.242)</t>
+  </si>
+  <si>
+    <t>0.066
+(0.592)</t>
+  </si>
+  <si>
+    <t>-0.233
+(0.683)</t>
+  </si>
+  <si>
+    <t>0.034
+(0.912)</t>
+  </si>
+  <si>
+    <t>0.062
+(0.860)</t>
+  </si>
+  <si>
+    <t>-0.135
+(0.812)</t>
+  </si>
+  <si>
+    <t>0.305
+(0.490)</t>
+  </si>
+  <si>
+    <t>-0.270
+(0.567)</t>
+  </si>
+  <si>
+    <t>0.177
+(0.686)</t>
+  </si>
+  <si>
+    <t>0.334
+(0.628)</t>
+  </si>
+  <si>
+    <t>Notes. p &lt; 0.10; *p &lt; 0.05; **p &lt; 0.01; ***p &lt; 0.001. Logit-3 refers to LowU and Logit-4 refers to LowJ.</t>
+  </si>
+  <si>
+    <t>0.002
+(0.942)</t>
+  </si>
+  <si>
+    <t>0.105
+(0.513)</t>
+  </si>
+  <si>
+    <t>0.003
+(0.988)</t>
+  </si>
+  <si>
+    <t>-0.178
+(0.366)</t>
+  </si>
+  <si>
+    <t>0.409
+(0.445)</t>
+  </si>
+  <si>
+    <t>0.738
+(0.265)</t>
+  </si>
+  <si>
+    <t>1.266
+(0.140)</t>
+  </si>
+  <si>
+    <t>1.119
+(0.186)</t>
+  </si>
+  <si>
+    <t>-0.230
+(0.824)</t>
+  </si>
+  <si>
+    <t>0.962
+(0.415)</t>
+  </si>
+  <si>
+    <t>1.563
+(0.162)</t>
+  </si>
+  <si>
+    <t>1.804
+(0.101)</t>
+  </si>
+  <si>
+    <t>0.674
+(0.441)</t>
+  </si>
+  <si>
+    <t>-1.003
+(0.374)</t>
+  </si>
+  <si>
+    <t>0.340
+(0.472)</t>
+  </si>
+  <si>
+    <t>0.901
+(0.217)</t>
+  </si>
+  <si>
+    <t>Table 2. Low(s) Purchase Behavior</t>
+  </si>
+  <si>
+    <t>3.683***
+(0.000)</t>
+  </si>
+  <si>
+    <t>-0.911***
+(0.000)</t>
+  </si>
+  <si>
+    <t>-0.457*
+(0.777)</t>
+  </si>
+  <si>
+    <t>-0.244*
+(0.015)</t>
+  </si>
+  <si>
+    <t>-0.686.
+(0.068)</t>
+  </si>
+  <si>
+    <t>-0.987**
+(0.002)</t>
+  </si>
+  <si>
+    <t>-1.180***
+(0.000)</t>
+  </si>
+  <si>
+    <t>1.385**
+(0.004)</t>
+  </si>
+  <si>
+    <t>-7.669**
+(0.001)</t>
+  </si>
+  <si>
+    <t>1.044.
+(0.069)</t>
+  </si>
+  <si>
+    <t>-4.484***
+(0.000)</t>
+  </si>
+  <si>
+    <t>0.599.
+(0.064)</t>
+  </si>
+  <si>
+    <t>1.407**
+(0.002)</t>
+  </si>
+  <si>
+    <t>1.147*
+(0.013)</t>
+  </si>
+  <si>
+    <t>0.952*
+(0.038)</t>
+  </si>
+  <si>
+    <t>ShapeRating.Explored (TRUE)</t>
+  </si>
+  <si>
+    <t>RF*ShapeRating.Explored</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +618,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -120,12 +626,353 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,18 +1269,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="139" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +1302,18 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="36"/>
+      <c r="K1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -466,8 +1329,26 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -483,8 +1364,26 @@
       <c r="E3">
         <v>0.33200000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -500,8 +1399,26 @@
       <c r="E4">
         <v>8.9999999999999993E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -517,8 +1434,26 @@
       <c r="E5">
         <v>0.85599999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -534,8 +1469,26 @@
       <c r="E6">
         <v>1.6E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -551,8 +1504,26 @@
       <c r="E7">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -568,8 +1539,26 @@
       <c r="E8">
         <v>0.65300000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -585,8 +1574,26 @@
       <c r="E9">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -602,8 +1609,26 @@
       <c r="E10">
         <v>0.46800000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -619,8 +1644,26 @@
       <c r="E11">
         <v>0.318</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -636,8 +1679,26 @@
       <c r="E12">
         <v>0.35699999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -653,8 +1714,26 @@
       <c r="E13">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -670,8 +1749,26 @@
       <c r="E14">
         <v>0.81799999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -687,8 +1784,26 @@
       <c r="E15">
         <v>0.747</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -704,8 +1819,26 @@
       <c r="E16">
         <v>0.78800000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -721,8 +1854,26 @@
       <c r="E17">
         <v>0.45600000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -738,8 +1889,26 @@
       <c r="E18">
         <v>0.55900000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -755,218 +1924,282 @@
       <c r="E19">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>-4.8920000000000003</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C24">
-        <v>0.33200000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="C25">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C26">
-        <v>0.85599999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="C27">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="C28">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="C29">
-        <v>0.65300000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30">
-        <v>-1.371</v>
-      </c>
-      <c r="C30">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31">
-        <v>-0.20599999999999999</v>
-      </c>
-      <c r="C31">
-        <v>0.46800000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32">
-        <v>-0.309</v>
-      </c>
-      <c r="C32">
-        <v>0.318</v>
-      </c>
+      <c r="G19" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="32" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="M20" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="34"/>
+      <c r="I21" s="35"/>
+      <c r="K21" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" s="34"/>
+      <c r="M21" s="35"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="C33">
-        <v>0.35699999999999998</v>
-      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="C34">
-        <v>2.5999999999999999E-2</v>
-      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35">
-        <v>-9.8000000000000004E-2</v>
-      </c>
-      <c r="C35">
-        <v>0.81799999999999995</v>
-      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36">
-        <v>0.13</v>
-      </c>
-      <c r="C36">
-        <v>0.747</v>
-      </c>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37">
-        <v>0.107</v>
-      </c>
-      <c r="C37">
-        <v>0.78800000000000003</v>
-      </c>
+      <c r="C37" s="37"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="C38">
-        <v>0.45600000000000002</v>
-      </c>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39">
-        <v>-0.22600000000000001</v>
-      </c>
-      <c r="C39">
-        <v>0.55900000000000005</v>
-      </c>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40">
-        <v>2.1890000000000001</v>
-      </c>
-      <c r="C40">
-        <v>1E-3</v>
-      </c>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G21:I21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275B46C5-4C05-284F-82D8-F72AB2CC6F4B}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>